<commit_message>
read time + computation time + total exec time
</commit_message>
<xml_diff>
--- a/ucv/src/main/resources/out/fork_join_metrics.xlsx
+++ b/ucv/src/main/resources/out/fork_join_metrics.xlsx
@@ -12,7 +12,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Execution Time (ms)</t>
+  </si>
   <si>
     <t>Fork-Join Multiplication Time</t>
   </si>
@@ -22,7 +31,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -30,16 +39,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -47,30 +71,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="23.4375" customWidth="true"/>
+    <col min="2" max="2" width="23.4375" customWidth="true"/>
+    <col min="3" max="3" width="23.4375" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="n" s="0">
-        <v>0.0011166</v>
+      <c r="B1" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>0.0856691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>